<commit_message>
descriptive statistics of new sample
</commit_message>
<xml_diff>
--- a/Descriptive Statistics/Categorical/Consideration_Offered_summary.xlsx
+++ b/Descriptive Statistics/Categorical/Consideration_Offered_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,36 +457,36 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C2" t="n">
-        <v>77.34999999999999</v>
+        <v>79.58</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Combinations</t>
+          <t>Common Equity</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" t="n">
-        <v>8.09</v>
+        <v>7.61</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Common Equity</t>
+          <t>Combinations</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" t="n">
-        <v>6.8</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
-        <v>6.15</v>
+        <v>4.84</v>
       </c>
     </row>
     <row r="6">
@@ -512,20 +512,33 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>1.29</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Cash; Unknown</t>
+          <t>Cash; Debt</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>0.32</v>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Debt</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>